<commit_message>
working model of MEPERS without risk-sharing
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_MEPERS_planInfo_AV2020.xlsx
+++ b/inputs/data_raw/Data_MEPERS_planInfo_AV2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_PewRiskSharing\model_MEPERS\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797050F6-AD18-4D9F-BC07-C6E8A790EC71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EB0E97-1244-4DAB-A373-C00FD4D796E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init_unrecReturn" sheetId="12" r:id="rId1"/>
@@ -756,7 +756,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0;&quot;$&quot;\-#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0;&quot;$&quot;\-#,##0"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -929,7 +929,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="10"/>
     </xf>
     <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -961,9 +961,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="15"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1022,6 +1019,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="15"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1405,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BFE154-32C8-48F8-AF28-84298376E385}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1498,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FFFA73-2D4A-4AA3-8BAA-C57267D0CB48}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1569,202 +1569,202 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="36">
-      <c r="C6" s="24"/>
-      <c r="D6" s="25" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
     </row>
     <row r="7" spans="1:10" ht="13.5" customHeight="1">
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="32" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="13.5" customHeight="1">
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="36">
         <v>2015</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="37">
         <v>15</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="38">
         <v>267090099</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="30" t="b">
+      <c r="J8" s="29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="13.5" customHeight="1">
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="34">
         <v>2016</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="37">
         <v>16</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="39">
         <v>111486515</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="30" t="b">
+      <c r="J9" s="29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="13.5" customHeight="1">
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="34">
         <v>2017</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="37">
         <v>17</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="39">
         <v>9687099</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="30" t="b">
+      <c r="J10" s="29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="13.5" customHeight="1">
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="34">
         <v>2018</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="37">
         <v>18</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="39">
         <v>-75544375</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="30" t="b">
+      <c r="J11" s="29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="13.5" customHeight="1">
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="34">
         <v>2019</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="37">
         <v>19</v>
       </c>
-      <c r="G12" s="40">
+      <c r="G12" s="39">
         <v>20708577</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="30" t="b">
+      <c r="J12" s="29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="13.5" customHeight="1">
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="34">
         <v>2020</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="37">
         <v>20</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="39">
         <v>12603412</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="30" t="b">
+      <c r="J13" s="29" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1808,10 +1808,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="43"/>
     </row>
     <row r="7" spans="1:4" ht="21.75" customHeight="1">
       <c r="C7" s="11" t="s">

</xml_diff>

<commit_message>
working model with simple risk sharing implementation.
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_MEPERS_planInfo_AV2020.xlsx
+++ b/inputs/data_raw/Data_MEPERS_planInfo_AV2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_PewRiskSharing\model_MEPERS\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EB0E97-1244-4DAB-A373-C00FD4D796E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E261F6C1-E37C-4A17-8133-813852680964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <t>year</t>
   </si>
@@ -747,6 +747,9 @@
   </si>
   <si>
     <t>C7:J13</t>
+  </si>
+  <si>
+    <t>C6:D9</t>
   </si>
 </sst>
 </file>
@@ -1403,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BFE154-32C8-48F8-AF28-84298376E385}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1424,7 +1427,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1432,7 +1435,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1440,7 +1443,7 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>20180630</v>
+        <v>20200630</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1453,38 +1456,30 @@
     </row>
     <row r="7" spans="1:4">
       <c r="C7">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="C8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="C10">
-        <v>2022</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="D11" s="1"/>
+      <c r="D10" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>